<commit_message>
added to do list
</commit_message>
<xml_diff>
--- a/comparator_tests.xlsx
+++ b/comparator_tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan\Documents\Grad School stuff\S20\Digital_IC\ECE725\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dylanrosser/Documents/Grad_School_Stuff/S20/digital/ECE725/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CD4BC3-7F59-4190-A9B8-178BCD6ED8D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA86EAFD-0312-A945-83A2-E2C81073A19F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3295" yWindow="0" windowWidth="14250" windowHeight="7470" xr2:uid="{2CB1362F-ACA9-48D4-AFEA-23BD9C03D6CB}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16680" activeTab="1" xr2:uid="{2CB1362F-ACA9-48D4-AFEA-23BD9C03D6CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="2" r:id="rId1"/>
@@ -25,9 +25,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="80">
   <si>
     <t>sndr</t>
   </si>
@@ -227,6 +225,54 @@
   </si>
   <si>
     <t>sigma^2_erf</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>V/V</t>
+  </si>
+  <si>
+    <t>fclk</t>
+  </si>
+  <si>
+    <t>Tmx</t>
+  </si>
+  <si>
+    <t>Vid_min</t>
+  </si>
+  <si>
+    <t>.noise</t>
+  </si>
+  <si>
+    <t>erf</t>
+  </si>
+  <si>
+    <t>V^2</t>
+  </si>
+  <si>
+    <t>noise typical - rf input and latch</t>
+  </si>
+  <si>
+    <t>pre simu, tran noise,  rf input &amp; latch, FMAX = 50G</t>
+  </si>
+  <si>
+    <t>pre simu, tran noise, nch for all, 50G</t>
+  </si>
+  <si>
+    <t>ummmmmmmm</t>
+  </si>
+  <si>
+    <t>100G</t>
+  </si>
+  <si>
+    <t>500G</t>
+  </si>
+  <si>
+    <t>pre simu, tran noise, nch, 200G</t>
+  </si>
+  <si>
+    <t>pre simu, tran noise, nch, 100G</t>
   </si>
 </sst>
 </file>
@@ -317,7 +363,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -335,16 +381,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -658,22 +694,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27D96E93-05FB-40DC-85F9-46A7B1BA943B}">
-  <dimension ref="A1:R22"/>
+  <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView topLeftCell="A20" zoomScale="189" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.40625" customWidth="1"/>
-    <col min="2" max="2" width="11.1796875" customWidth="1"/>
-    <col min="3" max="3" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.81640625" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>35</v>
       </c>
@@ -729,13 +765,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="3">
         <v>2.2000000000000001E-3</v>
       </c>
       <c r="C2" s="3">
-        <v>5.0000000000000002E-5</v>
+        <v>5.5000000000000003E-4</v>
       </c>
       <c r="D2" s="2">
         <v>0.42</v>
@@ -753,14 +789,14 @@
         <v>1.13E-4</v>
       </c>
       <c r="I2" s="3">
-        <f>0.00000000000000167+0.00000000000002</f>
-        <v>2.1670000000000001E-14</v>
+        <f>0.000000000000003305+0.000000000000000424</f>
+        <v>3.7289999999999997E-15</v>
       </c>
       <c r="J2" s="3">
-        <v>5.7499999999999998E-16</v>
+        <v>3.0200000000000003E-17</v>
       </c>
       <c r="K2" s="3">
-        <v>1000000000</v>
+        <v>380000000</v>
       </c>
       <c r="L2" s="2">
         <v>0.9</v>
@@ -776,7 +812,7 @@
       </c>
       <c r="P2" s="3">
         <f>1/(2*K2)</f>
-        <v>5.0000000000000003E-10</v>
+        <v>1.3157894736842105E-9</v>
       </c>
       <c r="Q2" s="2">
         <f>E2/2^10</f>
@@ -784,10 +820,10 @@
       </c>
       <c r="R2" s="3">
         <f>K2/10</f>
-        <v>100000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.75">
+        <v>38000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>33</v>
@@ -795,8 +831,20 @@
       <c r="C4" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="K4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L4" t="s">
+        <v>67</v>
+      </c>
+      <c r="M4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -805,57 +853,137 @@
         <v>8.176991150442479</v>
       </c>
       <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="K5" s="1">
+        <v>2000000000</v>
+      </c>
+      <c r="L5" s="1">
+        <f>1/(2*K5)</f>
+        <v>2.5000000000000002E-10</v>
+      </c>
+      <c r="M5" s="1">
+        <f>$L$2*EXP(-L5/$G$12)/$B$5</f>
+        <v>9.0346800433447044E-3</v>
+      </c>
+      <c r="N5" s="1">
+        <f>M5/$B$10</f>
+        <v>1.0038533381494116E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="3">
         <f>J2/(C2*(1-J2/I2))</f>
-        <v>1.181346290590187E-11</v>
+        <v>5.5357413215096787E-14</v>
       </c>
       <c r="C6" s="3">
         <f>P2/20</f>
-        <v>2.5000000000000001E-11</v>
-      </c>
-      <c r="E6">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.75">
+        <v>6.5789473684210521E-11</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="K6" s="1">
+        <v>1000000000</v>
+      </c>
+      <c r="L6" s="1">
+        <f t="shared" ref="L6:L15" si="0">1/(2*K6)</f>
+        <v>5.0000000000000003E-10</v>
+      </c>
+      <c r="M6" s="1">
+        <f t="shared" ref="M6:M15" si="1">$L$2*EXP(-L6/$G$12)/$B$5</f>
+        <v>7.4161169892531594E-4</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" ref="N6:N15" si="2">M6/$B$10</f>
+        <v>8.2401299880590652E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="3">
         <f>K2*(2*I2+J2)*L2^2</f>
-        <v>3.5571150000000006E-5</v>
+        <v>2.30486796E-6</v>
       </c>
       <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="1">
+        <f>L2*(EXP(-P2/G12))/B5</f>
+        <v>2.1244567986389459E-7</v>
+      </c>
+      <c r="K7" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="L7" s="1">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-9</v>
+      </c>
+      <c r="M7" s="1">
+        <f t="shared" si="1"/>
+        <v>2.1228772677265194E-23</v>
+      </c>
+      <c r="N7" s="1">
+        <f t="shared" si="2"/>
+        <v>2.3587525196961325E-23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B8" s="3">
         <f>10/(2*PI()*B6)</f>
-        <v>134723361269.77922</v>
+        <v>28750429951176.156</v>
       </c>
       <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="K8" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="L8" s="1">
+        <f t="shared" si="0"/>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="M8" s="1">
+        <f t="shared" si="1"/>
+        <v>7.8416603957319234E-219</v>
+      </c>
+      <c r="N8" s="1">
+        <f t="shared" si="2"/>
+        <v>8.7129559952576928E-219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="3" t="e">
         <f>L2/(B5*(EXP(P2/B6)))</f>
-        <v>4.5741682919312107E-20</v>
+        <v>#NUM!</v>
       </c>
       <c r="C9" s="3">
         <f>C11*B10</f>
         <v>9.0000000000000012E-9</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="K9" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="L9" s="1">
+        <f t="shared" si="0"/>
+        <v>4.9999999999999998E-7</v>
+      </c>
+      <c r="M9" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N9" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>56</v>
       </c>
@@ -864,108 +992,226 @@
         <v>0.9</v>
       </c>
       <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="K10" s="1">
+        <v>100000</v>
+      </c>
+      <c r="L10" s="1">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="M10" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="3" t="e">
         <f>B9/B10</f>
-        <v>5.0824092132569004E-20</v>
+        <v>#NUM!</v>
       </c>
       <c r="C11" s="3">
         <v>1E-8</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11">
+        <v>8.18</v>
+      </c>
+      <c r="H11" t="s">
+        <v>65</v>
+      </c>
+      <c r="K11" s="1">
+        <v>10000</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="M11" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B12" s="3">
         <f>-1/(LN((C11*B10*B5)/L2)*B6)</f>
-        <v>5187041808.4791737</v>
+        <v>1106932611856.9382</v>
       </c>
       <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1E-10</v>
+      </c>
+      <c r="H12" t="s">
+        <v>64</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1000</v>
+      </c>
+      <c r="L12" s="1">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="M12" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B13" s="3">
         <f>K2*(2*I2+J2)*L2^2</f>
-        <v>3.5571150000000006E-5</v>
+        <v>2.30486796E-6</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="F13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="1">
+        <f>G7/B10</f>
+        <v>2.3605075540432732E-7</v>
+      </c>
+      <c r="K13" s="1">
+        <v>100</v>
+      </c>
+      <c r="L13" s="1">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M13" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B14" s="3">
         <f>B13/R2</f>
-        <v>3.5571150000000006E-13</v>
+        <v>6.0654419999999998E-14</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="F14" t="s">
+        <v>57</v>
+      </c>
       <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="K14" s="1">
+        <v>10</v>
+      </c>
+      <c r="L14" s="1">
+        <f t="shared" si="0"/>
+        <v>0.05</v>
+      </c>
+      <c r="M14" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B15" s="3">
         <f>B14/10</f>
-        <v>3.5571150000000008E-14</v>
+        <v>6.0654419999999998E-15</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="K15" s="1">
+        <v>1</v>
+      </c>
+      <c r="L15" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="M15" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>59</v>
       </c>
       <c r="B16" s="3">
         <f>8*N2*O2*M2*B2*D2/(I2*H2)+2*N2*O2/(I2)</f>
-        <v>8.6304792319221143E-6</v>
+        <v>5.015352238019637E-5</v>
       </c>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>57</v>
       </c>
       <c r="B17" s="3">
         <f>B16/(B5^2)</f>
-        <v>1.2907670081193832E-7</v>
+        <v>7.500917421814706E-7</v>
       </c>
       <c r="C17" s="2">
         <f>Q2/6</f>
         <v>1.4648437499999999E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>57</v>
       </c>
       <c r="B18" s="3">
         <f>((G2-D2)/D2)*((4*N2*O2*M2/I2)+((G2-D2)/D2)*(N2*O2/(2*I2)))</f>
-        <v>2.3370181667498563E-7</v>
+        <v>1.3580902030965242E-6</v>
       </c>
       <c r="C18" s="2">
         <f>(0.00047)^2</f>
         <v>2.209E-7</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>62</v>
       </c>
@@ -974,13 +1220,63 @@
       </c>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>63</v>
       </c>
       <c r="B22" s="1">
         <f>B21^2</f>
         <v>1.6E-7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1.122E-6</v>
+      </c>
+      <c r="D25">
+        <f>SQRT(B25)</f>
+        <v>1.0592450141492288E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="1">
+        <v>3.2000000000000001E-7</v>
+      </c>
+      <c r="C26" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26">
+        <f>SQRT(B26)</f>
+        <v>5.6568542494923803E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="1">
+        <f>(0.0006)^2</f>
+        <v>3.5999999999999994E-7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B28" s="1">
+        <v>9.9669999999999992E-7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B29" s="1">
+        <v>5.3099999999999998E-7</v>
+      </c>
+      <c r="D29">
+        <f>SQRT(B29)</f>
+        <v>7.2869746808946719E-4</v>
       </c>
     </row>
   </sheetData>
@@ -998,15 +1294,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F17737-4689-4D57-98F3-165EFA539F96}">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:Y54"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1050,7 +1346,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0.1</v>
       </c>
@@ -1095,7 +1391,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0.2</v>
       </c>
@@ -1133,11 +1429,11 @@
         <v>52.935499999999998</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M30" si="0">(L3-1.76)/6.02</f>
+        <f t="shared" ref="M3:M25" si="0">(L3-1.76)/6.02</f>
         <v>8.500913621262459</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0.4</v>
       </c>
@@ -1179,7 +1475,7 @@
         <v>7.7958305647840538</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0.2</v>
       </c>
@@ -1221,7 +1517,7 @@
         <v>7.7367275747508311</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.2</v>
       </c>
@@ -1263,7 +1559,7 @@
         <v>8.4460465116279089</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.2</v>
       </c>
@@ -1305,7 +1601,7 @@
         <v>8.4862956810631225</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.4</v>
       </c>
@@ -1347,7 +1643,7 @@
         <v>8.5939202657807314</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0.5</v>
       </c>
@@ -1389,7 +1685,7 @@
         <v>8.3079235880398681</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0.4</v>
       </c>
@@ -1431,7 +1727,7 @@
         <v>8.3078737541528245</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0.4</v>
       </c>
@@ -1473,7 +1769,7 @@
         <v>8.5939368770764126</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0.4</v>
       </c>
@@ -1515,7 +1811,7 @@
         <v>8.5370265780730907</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>0.4</v>
       </c>
@@ -1557,7 +1853,7 @@
         <v>8.5799003322259146</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>0.5</v>
       </c>
@@ -1599,7 +1895,7 @@
         <v>8.5623421926910321</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0.5</v>
       </c>
@@ -1641,7 +1937,7 @@
         <v>8.5941196013289041</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0.5</v>
       </c>
@@ -1683,7 +1979,7 @@
         <v>8.5941694352159477</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>0.5</v>
       </c>
@@ -1725,7 +2021,7 @@
         <v>8.5941528239202665</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>0.6</v>
       </c>
@@ -1767,7 +2063,7 @@
         <v>8.5943687707641203</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>0.8</v>
       </c>
@@ -1809,7 +2105,7 @@
         <v>8.6357142857142861</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1851,7 +2147,7 @@
         <v>8.6360963455149502</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1893,7 +2189,7 @@
         <v>8.6656976744186061</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1.2</v>
       </c>
@@ -1935,7 +2231,7 @@
         <v>8.7441528239202668</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1.4</v>
       </c>
@@ -1977,7 +2273,7 @@
         <v>8.7993521594684392</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1.6</v>
       </c>
@@ -2019,7 +2315,7 @@
         <v>8.8565448504983397</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2</v>
       </c>
@@ -2065,6 +2361,343 @@
       </c>
       <c r="O25" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>0.2</v>
+      </c>
+      <c r="B29">
+        <v>0.2</v>
+      </c>
+      <c r="C29">
+        <v>2.4</v>
+      </c>
+      <c r="D29">
+        <v>2.4</v>
+      </c>
+      <c r="E29">
+        <v>0.2</v>
+      </c>
+      <c r="F29">
+        <v>0.2</v>
+      </c>
+      <c r="G29">
+        <v>2.4</v>
+      </c>
+      <c r="H29">
+        <v>2.4</v>
+      </c>
+      <c r="I29">
+        <v>12</v>
+      </c>
+      <c r="J29">
+        <v>12</v>
+      </c>
+      <c r="K29">
+        <v>0.2</v>
+      </c>
+      <c r="L29">
+        <v>58.097000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>0.2</v>
+      </c>
+      <c r="B33">
+        <v>0.2</v>
+      </c>
+      <c r="C33">
+        <v>2.4</v>
+      </c>
+      <c r="D33">
+        <v>2.4</v>
+      </c>
+      <c r="E33">
+        <v>0.2</v>
+      </c>
+      <c r="F33">
+        <v>0.2</v>
+      </c>
+      <c r="G33">
+        <v>2.4</v>
+      </c>
+      <c r="H33">
+        <v>2.4</v>
+      </c>
+      <c r="I33">
+        <v>12</v>
+      </c>
+      <c r="J33">
+        <v>12</v>
+      </c>
+      <c r="K33">
+        <v>0.2</v>
+      </c>
+      <c r="L33">
+        <v>54.09</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>0.2</v>
+      </c>
+      <c r="B34">
+        <v>0.2</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+      <c r="E34">
+        <v>0.2</v>
+      </c>
+      <c r="F34">
+        <v>0.2</v>
+      </c>
+      <c r="G34">
+        <v>0.3</v>
+      </c>
+      <c r="H34">
+        <v>0.3</v>
+      </c>
+      <c r="I34">
+        <v>13</v>
+      </c>
+      <c r="J34">
+        <v>13</v>
+      </c>
+      <c r="K34">
+        <v>0.2</v>
+      </c>
+      <c r="L34">
+        <v>53.805599999999998</v>
+      </c>
+      <c r="W34">
+        <v>-2.008</v>
+      </c>
+      <c r="X34">
+        <v>5.7960000000000003</v>
+      </c>
+      <c r="Y34">
+        <v>9.1769999999999996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="W36">
+        <f>W34-X34-Y34</f>
+        <v>-16.981000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>0.2</v>
+      </c>
+      <c r="B38">
+        <v>0.2</v>
+      </c>
+      <c r="C38">
+        <v>2.4</v>
+      </c>
+      <c r="D38">
+        <v>2.4</v>
+      </c>
+      <c r="E38">
+        <v>0.2</v>
+      </c>
+      <c r="F38">
+        <v>0.2</v>
+      </c>
+      <c r="G38">
+        <v>2.4</v>
+      </c>
+      <c r="H38">
+        <v>2.4</v>
+      </c>
+      <c r="I38">
+        <v>12</v>
+      </c>
+      <c r="J38">
+        <v>12</v>
+      </c>
+      <c r="K38">
+        <v>0.2</v>
+      </c>
+      <c r="L38">
+        <v>52.573</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="L39">
+        <v>52.659199999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="L41">
+        <v>53.386899999999997</v>
+      </c>
+      <c r="M41" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="M42" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="L43">
+        <v>52.652000000000001</v>
+      </c>
+      <c r="M43" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="L46">
+        <v>52.894599999999997</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>0.2</v>
+      </c>
+      <c r="B50">
+        <v>0.2</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
+      </c>
+      <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="E50">
+        <v>0.2</v>
+      </c>
+      <c r="F50">
+        <v>0.2</v>
+      </c>
+      <c r="G50">
+        <v>2</v>
+      </c>
+      <c r="H50">
+        <v>2</v>
+      </c>
+      <c r="I50">
+        <v>14</v>
+      </c>
+      <c r="J50">
+        <v>14</v>
+      </c>
+      <c r="K50">
+        <v>0.2</v>
+      </c>
+      <c r="L50">
+        <v>53.972499999999997</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>0.2</v>
+      </c>
+      <c r="B52">
+        <v>0.2</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
+      <c r="E52">
+        <v>0.2</v>
+      </c>
+      <c r="F52">
+        <v>0.2</v>
+      </c>
+      <c r="G52">
+        <v>2</v>
+      </c>
+      <c r="H52">
+        <v>2</v>
+      </c>
+      <c r="I52">
+        <v>16</v>
+      </c>
+      <c r="J52">
+        <v>16</v>
+      </c>
+      <c r="K52">
+        <v>0.2</v>
+      </c>
+      <c r="L52">
+        <v>53.748699999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>0.2</v>
+      </c>
+      <c r="B54">
+        <v>0.2</v>
+      </c>
+      <c r="C54">
+        <v>4</v>
+      </c>
+      <c r="D54">
+        <v>4</v>
+      </c>
+      <c r="E54">
+        <v>0.2</v>
+      </c>
+      <c r="F54">
+        <v>0.2</v>
+      </c>
+      <c r="G54">
+        <v>4</v>
+      </c>
+      <c r="H54">
+        <v>4</v>
+      </c>
+      <c r="I54">
+        <v>16</v>
+      </c>
+      <c r="J54">
+        <v>16</v>
+      </c>
+      <c r="K54">
+        <v>0.2</v>
+      </c>
+      <c r="L54">
+        <v>55.118600000000001</v>
       </c>
     </row>
   </sheetData>
@@ -2080,9 +2713,9 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -2117,7 +2750,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>0.1</v>
       </c>
@@ -2152,7 +2785,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>36</v>
       </c>
@@ -2167,7 +2800,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>6.3400000000000005E-17</v>
       </c>
@@ -2183,7 +2816,7 @@
         <v>1.6654E-15</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -2209,7 +2842,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>6.8599999999999996E-17</v>
       </c>

</xml_diff>